<commit_message>
Se realiza las pruebas unitarias y funcionales de SVM
</commit_message>
<xml_diff>
--- a/pruebas-funcionales/Serguros-de-viaje-mundial/pruebas-funcionales.xlsx
+++ b/pruebas-funcionales/Serguros-de-viaje-mundial/pruebas-funcionales.xlsx
@@ -8,20 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crist\OneDrive\Documentos\Cristian\Prueba-tecnica\prueba-tecnica\pruebas-funcionales\Serguros-de-viaje-mundial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A5FD9AE-5700-4CED-AAA7-7E64AFB46B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEB10AEB-B1E8-4CD2-AD1D-850BA0FA6B0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PF-1" sheetId="1" r:id="rId1"/>
     <sheet name="PF-2" sheetId="3" r:id="rId2"/>
     <sheet name="PF-3" sheetId="4" r:id="rId3"/>
-    <sheet name="PF-4" sheetId="5" r:id="rId4"/>
-    <sheet name="PF-5" sheetId="7" r:id="rId5"/>
-    <sheet name="Parametrización" sheetId="2" r:id="rId6"/>
+    <sheet name="PF-6" sheetId="7" r:id="rId4"/>
+    <sheet name="Parametrización" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -38,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="88">
   <si>
     <t>Estado</t>
   </si>
@@ -109,15 +107,6 @@
     <t>Servicios</t>
   </si>
   <si>
-    <t>Mi Asistencia</t>
-  </si>
-  <si>
-    <t>Ayuda</t>
-  </si>
-  <si>
-    <t>Cotizar Gratis</t>
-  </si>
-  <si>
     <t>Se debe desplegar con las siguientes opciones:
 1. Planes y beneficios
 2. Beneficios Adicionales
@@ -134,9 +123,6 @@
 2. Contactos</t>
   </si>
   <si>
-    <t>Botón que permite validar el formulario de cotización.</t>
-  </si>
-  <si>
     <t>Debe validar las resticciones de cada campo y notificar por medio de una modal.</t>
   </si>
   <si>
@@ -149,99 +135,6 @@
     <t>Se genera la modal, pero hace falta validacioes importantes en cuando a los campos, así mismo se puede dejar mas limpia la data que ingresa al sistema.</t>
   </si>
   <si>
-    <t>Botón continuar</t>
-  </si>
-  <si>
-    <t>Lista de planes</t>
-  </si>
-  <si>
-    <t>Lista de beneficios</t>
-  </si>
-  <si>
-    <t>Permite redireccionar a la confirmación de datos.</t>
-  </si>
-  <si>
-    <t>Para redireccionar debe tener seleccionado un plan.</t>
-  </si>
-  <si>
-    <t>Redirecciona correctamente con el plan seleccionado.</t>
-  </si>
-  <si>
-    <t>Se debe listar los planes en forma de card, con su respectiva imagen y un botón de detalle.</t>
-  </si>
-  <si>
-    <t>Botón ver detalle</t>
-  </si>
-  <si>
-    <t>Este botón debe mostrar todo el detalle del plan, en una modal.</t>
-  </si>
-  <si>
-    <t>Se muestra la lista de los planes.</t>
-  </si>
-  <si>
-    <t>Check plan</t>
-  </si>
-  <si>
-    <t>Selección para el plan.</t>
-  </si>
-  <si>
-    <t>Debe desplegar una modal con toda la información de plan.</t>
-  </si>
-  <si>
-    <t>Se despliega una modal, mostrando toda la información.</t>
-  </si>
-  <si>
-    <t>Al seleccionar el plan, el valor debe estar actualizando según el plan seleccionado.</t>
-  </si>
-  <si>
-    <t>Se cambia los valores al seleccionar el plan</t>
-  </si>
-  <si>
-    <t>En este momento se lista los planes, pero no se puede aplicar la tecnica de caja blanca ya que no tenemos acceso al código del sistema.</t>
-  </si>
-  <si>
-    <t>En el sistema muestra que cambia los valores, pero para realizar la tecnica de caja blanca y evidenciar que los valores cambian según la divisa, se debe tener una mejor documentación y tener acceso al código.</t>
-  </si>
-  <si>
-    <t>Se debe listar los beneficios en forma de card, con su respectiva imagen y un check.</t>
-  </si>
-  <si>
-    <t>Se muestra la lista de los beneficios.</t>
-  </si>
-  <si>
-    <t>Check del beneficio</t>
-  </si>
-  <si>
-    <t>Selecciona el beneficio a convenir</t>
-  </si>
-  <si>
-    <t>Al seleccionar el beneficio, el valor debe estar actualizando según el beneficio seleccionado.</t>
-  </si>
-  <si>
-    <t>Se cambia los valores al seleccionar el benficio</t>
-  </si>
-  <si>
-    <t>SVP-PF-Cotizar</t>
-  </si>
-  <si>
-    <t>SVP-PF-Home</t>
-  </si>
-  <si>
-    <t>SVP-PF-Cotizar-completa-datos</t>
-  </si>
-  <si>
-    <t>Botón Anterior</t>
-  </si>
-  <si>
-    <t>Formulario</t>
-  </si>
-  <si>
-    <t>Permite redireccionar a la selección de plan.</t>
-  </si>
-  <si>
-    <t>Redirecciona correctamente a la selección del plan.</t>
-  </si>
-  <si>
     <t>Permite redireccionar a los metodos de pago.</t>
   </si>
   <si>
@@ -251,95 +144,19 @@
     <t>Redirecciona correctamente a los metodos de pago, con el formulario completado.</t>
   </si>
   <si>
-    <t>Muestra la lista de viajeros con datos que se deben ingresar para poder continuar con la compra</t>
-  </si>
-  <si>
     <t>Los campos a deligenciar deben estar macado con un *, y en caso de estar vacios el color del campo debe colocarce rojo.</t>
   </si>
   <si>
     <t>Se agregan los datos faltantes al formulario.</t>
   </si>
   <si>
-    <t>Este formulario tiene su pruebas unitarias y se encuentra en el trello: 
-https://trello.com/b/Pw09izMe/seguro-para-viaje</t>
-  </si>
-  <si>
-    <t>Lista de método de pago</t>
-  </si>
-  <si>
-    <t>Check Acepto términos y condiciones</t>
-  </si>
-  <si>
-    <t>Check Acepto políticas de privacidad</t>
-  </si>
-  <si>
-    <t>Inscribase a nuestro boletín</t>
-  </si>
-  <si>
     <t>Permite redireccionar al pago que seleccione.</t>
-  </si>
-  <si>
-    <t>Para redireccionar debe tener chequeado los términos y condiciones, políticas de privacidad</t>
   </si>
   <si>
     <t>Redirecciona correctamente al pago seleccionado.</t>
   </si>
   <si>
-    <t>Check de métodos de pagos</t>
-  </si>
-  <si>
-    <t>Selección para el método de pago</t>
-  </si>
-  <si>
-    <t>Lo debe redireccinar al pago seleccionado cuando le da el botón continuar.</t>
-  </si>
-  <si>
     <t>Home</t>
-  </si>
-  <si>
-    <t>Cotizador</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Completar datos </t>
-  </si>
-  <si>
-    <t>SVP-PF-Cotizar-metodo-de-pago</t>
-  </si>
-  <si>
-    <t>Método de pago</t>
-  </si>
-  <si>
-    <t>Se debe chequear los términos y condiciones</t>
-  </si>
-  <si>
-    <t>Se debe chequear los políticas de privacidad</t>
-  </si>
-  <si>
-    <t>Se debe chequear a nuestro boletín</t>
-  </si>
-  <si>
-    <t>Este campo es requerido.</t>
-  </si>
-  <si>
-    <t>Si no se chequea debe salir una modal, notificando que los términos y condiciones deben ser requeridos.</t>
-  </si>
-  <si>
-    <t>Si no se chequea debe salir una modal, notificando que las polítcas de privacidad deben ser requeridos.</t>
-  </si>
-  <si>
-    <t>Este check no se selecciona.</t>
-  </si>
-  <si>
-    <t>Correo al cliente</t>
-  </si>
-  <si>
-    <t>Al correo del cliente llega el enlace y el resumen de la cotización realizada.</t>
-  </si>
-  <si>
-    <t>Debe llegar el correo con el enlace correspondiente</t>
-  </si>
-  <si>
-    <t>Llega el correo y se seleccioan el enlace correspondiente, abriendo el detalle de la cotización y seguir con la compra.</t>
   </si>
   <si>
     <t>Compra exitosa</t>
@@ -365,6 +182,133 @@
   </si>
   <si>
     <t>Para comprobar este caso se requiere la compra exitosa.</t>
+  </si>
+  <si>
+    <t>Nosotros</t>
+  </si>
+  <si>
+    <t>Solicita asistencia</t>
+  </si>
+  <si>
+    <t>Cotizar gratis</t>
+  </si>
+  <si>
+    <t>Botón que permite validar el formulario de la cotización.</t>
+  </si>
+  <si>
+    <t>SVM-PF-Home</t>
+  </si>
+  <si>
+    <t>Correo de la cotización</t>
+  </si>
+  <si>
+    <t>SVM-PF-email-cotización</t>
+  </si>
+  <si>
+    <t>Email del Cliente</t>
+  </si>
+  <si>
+    <t>Al solicitar la cotización, el cliente recibe un email con los datos correspondiente</t>
+  </si>
+  <si>
+    <t>En el email debe llegar un enlace para redireccionar a la solicitud de compra.</t>
+  </si>
+  <si>
+    <t>El email llega con un enlace donde lo redireccioan a la solicitud de compra.</t>
+  </si>
+  <si>
+    <t>Datos de la cotización</t>
+  </si>
+  <si>
+    <t>SVM-PF-datos-de-la-cotización</t>
+  </si>
+  <si>
+    <t>Información de los pasajeros</t>
+  </si>
+  <si>
+    <t>Datos de contacto</t>
+  </si>
+  <si>
+    <t>Editar datos de viaje</t>
+  </si>
+  <si>
+    <t>Ver detalle de cobertura</t>
+  </si>
+  <si>
+    <t>Muestran los datos que se realizo en la cotización inicial, agregar más pasajeros</t>
+  </si>
+  <si>
+    <t>Al agregar más pasajeros se debe actualizar y calcular el valor de la cotización</t>
+  </si>
+  <si>
+    <t>Se agrega los pasajeros 5 pasajeros</t>
+  </si>
+  <si>
+    <t>Se muestra los datos del contacto donde podra editarlo o agregar los datos a los campos requeridos.</t>
+  </si>
+  <si>
+    <t>Calcular valor de la cotización</t>
+  </si>
+  <si>
+    <t>El usuario visualiza los datos correctos que corresponden al calculo de su cotizacion</t>
+  </si>
+  <si>
+    <t>Muestra los valores de la cotización y se actualza dependiendo de la acción 1</t>
+  </si>
+  <si>
+    <t>El usuario modifica los datos de su solicitud de cotizacion correctamente</t>
+  </si>
+  <si>
+    <t>Muestra una modal donde podrá editar los datos de su viaje.</t>
+  </si>
+  <si>
+    <t>Despliega una modal donde muestra toda la información que tenga la cobertura</t>
+  </si>
+  <si>
+    <t>Muestra toda la información solicitada.</t>
+  </si>
+  <si>
+    <t>Botón Paga aquí</t>
+  </si>
+  <si>
+    <t>Si las acciones 1 y 2, cumple con las validaciones, este botón despliega las formas de pago</t>
+  </si>
+  <si>
+    <t>Redirecciona correctamente a la forma de pago, con el formulario completado.</t>
+  </si>
+  <si>
+    <t>Forma de pago</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> check Acepto terminos y condiciones</t>
+  </si>
+  <si>
+    <t>El usuario acepta los terminos y vondiciones, al darle click lo redirecciona al archivo PDF del mismo</t>
+  </si>
+  <si>
+    <t>El campo es requerido</t>
+  </si>
+  <si>
+    <t>Debe redireccionar a los terminos y condiciones del sistema.</t>
+  </si>
+  <si>
+    <t>Botón finaliza tu pago</t>
+  </si>
+  <si>
+    <t>Para redireccionar debe aceptar los terminos y condiciones.</t>
+  </si>
+  <si>
+    <t>Este caso se debe definir con un test de caja blanca donde se conozcan los detalles del código que calcula la cotización y se verifique que son correctos:
+https://trello.com/c/EOPwjUKv/2-svm-datos-de-cotizaci%C3%B3n</t>
+  </si>
+  <si>
+    <t>Formas de pago</t>
+  </si>
+  <si>
+    <t>El usuario completa la compra dependiendo de la  forma de pago que elija</t>
+  </si>
+  <si>
+    <t>El usuario seleccioan la forma de pago</t>
   </si>
 </sst>
 </file>
@@ -574,7 +518,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
@@ -613,20 +557,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -652,9 +599,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -667,23 +611,29 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -905,8 +855,8 @@
   </sheetPr>
   <dimension ref="A1:AA973"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -917,18 +867,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="25"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="26"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
@@ -948,16 +898,16 @@
       <c r="AA1" s="5"/>
     </row>
     <row r="2" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="26"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="28"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="29"/>
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
@@ -977,16 +927,16 @@
       <c r="AA2" s="5"/>
     </row>
     <row r="3" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="21"/>
+      <c r="B3" s="22"/>
       <c r="C3" s="15"/>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="37"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="21"/>
       <c r="G3" s="7" t="s">
         <v>0</v>
       </c>
@@ -1016,24 +966,24 @@
       <c r="AA3" s="5"/>
     </row>
     <row r="4" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="23" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="15"/>
-      <c r="C4" s="29" t="s">
-        <v>59</v>
+      <c r="C4" s="19" t="s">
+        <v>50</v>
       </c>
       <c r="D4" s="15"/>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="23" t="s">
         <v>4</v>
       </c>
       <c r="F4" s="15"/>
-      <c r="G4" s="35" t="s">
+      <c r="G4" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="36"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
@@ -1085,7 +1035,7 @@
     </row>
     <row r="6" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="30" t="s">
-        <v>82</v>
+        <v>37</v>
       </c>
       <c r="B6" s="31"/>
       <c r="C6" s="31"/>
@@ -1121,19 +1071,19 @@
       <c r="B7" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="34" t="s">
+      <c r="C7" s="34"/>
+      <c r="D7" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="20"/>
-      <c r="F7" s="34" t="s">
+      <c r="E7" s="34"/>
+      <c r="F7" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="20"/>
+      <c r="G7" s="34"/>
       <c r="H7" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="20"/>
+      <c r="I7" s="34"/>
       <c r="J7" s="12" t="s">
         <v>8</v>
       </c>
@@ -1160,19 +1110,19 @@
         <v>1</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="C8" s="15"/>
-      <c r="D8" s="16" t="s">
-        <v>26</v>
+      <c r="D8" s="17" t="s">
+        <v>23</v>
       </c>
       <c r="E8" s="15"/>
-      <c r="F8" s="17" t="s">
-        <v>32</v>
+      <c r="F8" s="16" t="s">
+        <v>28</v>
       </c>
       <c r="G8" s="15"/>
-      <c r="H8" s="17" t="s">
-        <v>32</v>
+      <c r="H8" s="16" t="s">
+        <v>28</v>
       </c>
       <c r="I8" s="15"/>
       <c r="J8" s="10" t="s">
@@ -1201,19 +1151,19 @@
         <v>2</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="15"/>
-      <c r="D9" s="16" t="s">
-        <v>27</v>
+      <c r="D9" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="E9" s="15"/>
-      <c r="F9" s="17" t="s">
-        <v>32</v>
+      <c r="F9" s="16" t="s">
+        <v>28</v>
       </c>
       <c r="G9" s="15"/>
-      <c r="H9" s="17" t="s">
-        <v>32</v>
+      <c r="H9" s="16" t="s">
+        <v>28</v>
       </c>
       <c r="I9" s="15"/>
       <c r="J9" s="10" t="s">
@@ -1242,19 +1192,19 @@
         <v>3</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="C10" s="15"/>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="15"/>
+      <c r="F10" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="17" t="s">
-        <v>32</v>
-      </c>
       <c r="G10" s="15"/>
-      <c r="H10" s="17" t="s">
-        <v>32</v>
+      <c r="H10" s="16" t="s">
+        <v>28</v>
       </c>
       <c r="I10" s="15"/>
       <c r="J10" s="10" t="s">
@@ -1283,19 +1233,19 @@
         <v>4</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="C11" s="15"/>
-      <c r="D11" s="16" t="s">
-        <v>29</v>
+      <c r="D11" s="17" t="s">
+        <v>49</v>
       </c>
       <c r="E11" s="15"/>
-      <c r="F11" s="17" t="s">
-        <v>30</v>
+      <c r="F11" s="16" t="s">
+        <v>26</v>
       </c>
       <c r="G11" s="15"/>
-      <c r="H11" s="17" t="s">
-        <v>31</v>
+      <c r="H11" s="16" t="s">
+        <v>27</v>
       </c>
       <c r="I11" s="15"/>
       <c r="J11" s="10" t="s">
@@ -1323,15 +1273,15 @@
       <c r="A12" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="20"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="34"/>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
@@ -1354,17 +1304,17 @@
       <c r="A13" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="20"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="34"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
@@ -1388,15 +1338,15 @@
         <v>4</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="21"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
       <c r="J14" s="15"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
@@ -29229,14 +29179,12 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="B13:J13"/>
+    <mergeCell ref="A12:J12"/>
     <mergeCell ref="G4:J4"/>
     <mergeCell ref="D3:F3"/>
     <mergeCell ref="B14:J14"/>
@@ -29253,14 +29201,16 @@
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="B13:J13"/>
-    <mergeCell ref="A12:J12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -29286,51 +29236,51 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6F91DAD-9DEA-4A7B-9E5D-F17669E7A5A9}">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B11" sqref="B11:J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="25"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="26"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="26"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="28"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="29"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="21"/>
+      <c r="B3" s="22"/>
       <c r="C3" s="15"/>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="37"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="21"/>
       <c r="G3" s="7" t="s">
         <v>0</v>
       </c>
@@ -29343,24 +29293,24 @@
       <c r="J3" s="8"/>
     </row>
     <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="23" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="15"/>
-      <c r="C4" s="29" t="s">
-        <v>58</v>
+      <c r="C4" s="19" t="s">
+        <v>52</v>
       </c>
       <c r="D4" s="15"/>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="23" t="s">
         <v>4</v>
       </c>
       <c r="F4" s="15"/>
-      <c r="G4" s="35" t="s">
+      <c r="G4" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="36"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="20"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="30" t="s">
@@ -29378,7 +29328,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="30" t="s">
-        <v>83</v>
+        <v>51</v>
       </c>
       <c r="B6" s="31"/>
       <c r="C6" s="31"/>
@@ -29397,184 +29347,429 @@
       <c r="B7" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="34" t="s">
+      <c r="C7" s="34"/>
+      <c r="D7" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="20"/>
-      <c r="F7" s="34" t="s">
+      <c r="E7" s="34"/>
+      <c r="F7" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="20"/>
+      <c r="G7" s="34"/>
       <c r="H7" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="20"/>
+      <c r="I7" s="34"/>
       <c r="J7" s="12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9">
         <v>1</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="C8" s="15"/>
-      <c r="D8" s="16" t="s">
-        <v>37</v>
+      <c r="D8" s="17" t="s">
+        <v>54</v>
       </c>
       <c r="E8" s="15"/>
-      <c r="F8" s="17" t="s">
-        <v>38</v>
+      <c r="F8" s="16" t="s">
+        <v>55</v>
       </c>
       <c r="G8" s="15"/>
-      <c r="H8" s="17" t="s">
-        <v>39</v>
+      <c r="H8" s="16" t="s">
+        <v>56</v>
       </c>
       <c r="I8" s="15"/>
       <c r="J8" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="34"/>
+    </row>
+    <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="A10" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="34"/>
+    </row>
+    <row r="11" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="20">
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A6:J6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="A1:J2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="A9:J9"/>
+    <mergeCell ref="B10:J10"/>
+    <mergeCell ref="B11:J11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{F3E50F5E-9655-4EB9-AAFD-74771D896252}">
+          <x14:formula1>
+            <xm:f>Parametrización!$B$1:$C$1</xm:f>
+          </x14:formula1>
+          <xm:sqref>H3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{812A606F-9D08-4C66-8867-6DA0E20FF5B6}">
+          <x14:formula1>
+            <xm:f>Parametrización!$B$2:$E$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>J8</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11221440-AA95-42F2-A26D-22C8159F662D}">
+  <dimension ref="A1:J19"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="26"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="27"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="29"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="22"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="17"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="8"/>
+    </row>
+    <row r="4" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="15"/>
+      <c r="C4" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="15"/>
+      <c r="E4" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="15"/>
+      <c r="G4" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="20"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="32"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="32"/>
+    </row>
+    <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="34"/>
+      <c r="D7" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="34"/>
+      <c r="F7" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="34"/>
+      <c r="H7" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="34"/>
+      <c r="J7" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="9">
+        <v>1</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="15"/>
+      <c r="D8" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" s="15"/>
+      <c r="F8" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="G8" s="15"/>
+      <c r="H8" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="I8" s="15"/>
+      <c r="J8" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9">
         <v>2</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="C9" s="15"/>
-      <c r="D9" s="16" t="s">
-        <v>40</v>
+      <c r="D9" s="17" t="s">
+        <v>66</v>
       </c>
       <c r="E9" s="15"/>
-      <c r="F9" s="17" t="s">
-        <v>14</v>
+      <c r="F9" s="16" t="s">
+        <v>33</v>
       </c>
       <c r="G9" s="15"/>
-      <c r="H9" s="17" t="s">
-        <v>43</v>
+      <c r="H9" s="16" t="s">
+        <v>34</v>
       </c>
       <c r="I9" s="15"/>
       <c r="J9" s="10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9">
         <v>3</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
-      <c r="C10" s="15"/>
+      <c r="C10" s="38"/>
       <c r="D10" s="16" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="17" t="s">
-        <v>46</v>
+      <c r="E10" s="21"/>
+      <c r="F10" s="16" t="s">
+        <v>14</v>
       </c>
-      <c r="G10" s="15"/>
-      <c r="H10" s="17" t="s">
-        <v>47</v>
+      <c r="G10" s="21"/>
+      <c r="H10" s="16" t="s">
+        <v>68</v>
       </c>
-      <c r="I10" s="15"/>
+      <c r="I10" s="21"/>
       <c r="J10" s="10" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="C11" s="15"/>
-      <c r="D11" s="16" t="s">
-        <v>45</v>
+      <c r="D11" s="17" t="s">
+        <v>71</v>
       </c>
       <c r="E11" s="15"/>
-      <c r="F11" s="17" t="s">
-        <v>48</v>
+      <c r="F11" s="16" t="s">
+        <v>33</v>
       </c>
       <c r="G11" s="15"/>
-      <c r="H11" s="17" t="s">
-        <v>49</v>
+      <c r="H11" s="16" t="s">
+        <v>70</v>
       </c>
       <c r="I11" s="15"/>
       <c r="J11" s="10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="C12" s="15"/>
-      <c r="D12" s="16" t="s">
-        <v>52</v>
+      <c r="D12" s="17" t="s">
+        <v>72</v>
       </c>
       <c r="E12" s="15"/>
-      <c r="F12" s="17" t="s">
+      <c r="F12" s="16" t="s">
         <v>14</v>
       </c>
       <c r="G12" s="15"/>
-      <c r="H12" s="17" t="s">
-        <v>53</v>
+      <c r="H12" s="16" t="s">
+        <v>73</v>
       </c>
       <c r="I12" s="15"/>
       <c r="J12" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="C13" s="15"/>
-      <c r="D13" s="16" t="s">
-        <v>55</v>
+      <c r="D13" s="17" t="s">
+        <v>75</v>
       </c>
       <c r="E13" s="15"/>
-      <c r="F13" s="17" t="s">
-        <v>56</v>
+      <c r="F13" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="G13" s="15"/>
-      <c r="H13" s="17" t="s">
-        <v>57</v>
+      <c r="H13" s="16" t="s">
+        <v>76</v>
       </c>
       <c r="I13" s="15"/>
       <c r="J13" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="9">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>34</v>
+        <v>77</v>
       </c>
       <c r="C14" s="15"/>
-      <c r="D14" s="16" t="s">
-        <v>37</v>
+      <c r="D14" s="17" t="s">
+        <v>30</v>
       </c>
       <c r="E14" s="15"/>
-      <c r="F14" s="17" t="s">
-        <v>38</v>
+      <c r="F14" s="16" t="s">
+        <v>31</v>
       </c>
       <c r="G14" s="15"/>
-      <c r="H14" s="17" t="s">
+      <c r="H14" s="16" t="s">
         <v>32</v>
       </c>
       <c r="I14" s="15"/>
@@ -29582,117 +29777,111 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="33" t="s">
-        <v>21</v>
+    <row r="15" spans="1:10" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="9">
+        <v>8</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="20"/>
-    </row>
-    <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="13" t="s">
+      <c r="B15" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" s="15"/>
+      <c r="D15" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="E15" s="15"/>
+      <c r="F15" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="G15" s="15"/>
+      <c r="H15" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="I15" s="15"/>
+      <c r="J15" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="9">
+        <v>9</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" s="15"/>
+      <c r="D16" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="15"/>
+      <c r="F16" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="G16" s="15"/>
+      <c r="H16" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="I16" s="15"/>
+      <c r="J16" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="A17" s="33"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="34"/>
+    </row>
+    <row r="18" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="A18" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B18" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="20"/>
-    </row>
-    <row r="17" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="9">
-        <v>2</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="21"/>
-      <c r="J17" s="15"/>
-    </row>
-    <row r="18" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="9">
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
+      <c r="J18" s="34"/>
+    </row>
+    <row r="19" spans="1:10" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="9">
         <v>3</v>
       </c>
-      <c r="B18" s="14" t="s">
-        <v>51</v>
+      <c r="B19" s="14" t="s">
+        <v>84</v>
       </c>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="15"/>
-    </row>
-    <row r="19" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="9">
-        <v>4</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="21"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22"/>
       <c r="J19" s="15"/>
     </row>
-    <row r="20" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="9">
-        <v>7</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="21"/>
-      <c r="J20" s="15"/>
-    </row>
   </sheetData>
-  <mergeCells count="47">
-    <mergeCell ref="B18:J18"/>
-    <mergeCell ref="B19:J19"/>
-    <mergeCell ref="B20:J20"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:I11"/>
+  <mergeCells count="52">
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="H15:I15"/>
     <mergeCell ref="A1:J2"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="D3:F3"/>
@@ -29710,378 +29899,30 @@
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="H8:I8"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B19:J19"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="F9:G9"/>
     <mergeCell ref="H9:I9"/>
-    <mergeCell ref="A15:J15"/>
-    <mergeCell ref="B16:J16"/>
-    <mergeCell ref="B17:J17"/>
+    <mergeCell ref="A17:J17"/>
+    <mergeCell ref="B18:J18"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="H12:I12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:I13"/>
     <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H14:I14"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{F3E50F5E-9655-4EB9-AAFD-74771D896252}">
-          <x14:formula1>
-            <xm:f>Parametrización!$B$1:$C$1</xm:f>
-          </x14:formula1>
-          <xm:sqref>H3</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{812A606F-9D08-4C66-8867-6DA0E20FF5B6}">
-          <x14:formula1>
-            <xm:f>Parametrización!$B$2:$E$2</xm:f>
-          </x14:formula1>
-          <xm:sqref>J8:J14</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11221440-AA95-42F2-A26D-22C8159F662D}">
-  <dimension ref="A1:J15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="25"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="26"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="28"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="8"/>
-    </row>
-    <row r="4" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="15"/>
-      <c r="G4" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="36"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="31"/>
-      <c r="J5" s="32"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="30" t="s">
-        <v>84</v>
-      </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="32"/>
-    </row>
-    <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="20"/>
-      <c r="F7" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" s="20"/>
-      <c r="H7" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="I7" s="20"/>
-      <c r="J7" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="9">
-        <v>1</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="E8" s="15"/>
-      <c r="F8" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="15"/>
-      <c r="H8" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="I8" s="15"/>
-      <c r="J8" s="10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="9">
-        <v>2</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="E9" s="15"/>
-      <c r="F9" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="G9" s="15"/>
-      <c r="H9" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="I9" s="15"/>
-      <c r="J9" s="10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9">
-        <v>3</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="G10" s="15"/>
-      <c r="H10" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="I10" s="15"/>
-      <c r="J10" s="10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9">
-        <v>3</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="C11" s="15"/>
-      <c r="D11" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="E11" s="15"/>
-      <c r="F11" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="15"/>
-      <c r="H11" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="I11" s="15"/>
-      <c r="J11" s="10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="9">
-        <v>3</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="15"/>
-      <c r="D12" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="E12" s="15"/>
-      <c r="F12" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="G12" s="15"/>
-      <c r="H12" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="I12" s="15"/>
-      <c r="J12" s="10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="20"/>
-    </row>
-    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="A14" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="20"/>
-    </row>
-    <row r="15" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="9">
-        <v>3</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="15"/>
-    </row>
-  </sheetData>
-  <mergeCells count="36">
-    <mergeCell ref="B15:J15"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="A13:J13"/>
-    <mergeCell ref="B14:J14"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="A5:J5"/>
-    <mergeCell ref="A6:J6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="A1:J2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:J4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -30091,7 +29932,7 @@
           <x14:formula1>
             <xm:f>Parametrización!$B$2:$E$2</xm:f>
           </x14:formula1>
-          <xm:sqref>J8:J12</xm:sqref>
+          <xm:sqref>J8:J16</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{BD34DE18-4CC0-43D0-A5A9-701E4E41D9CE}">
           <x14:formula1>
@@ -30106,52 +29947,52 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A44D7B4-0AC4-4799-BEDB-3821EB010498}">
-  <dimension ref="A1:J19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4E67FA-54D1-424D-A222-EDE2699A7FA4}">
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="25"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="26"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="26"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="28"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="29"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="21"/>
+      <c r="B3" s="22"/>
       <c r="C3" s="15"/>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="37"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="21"/>
       <c r="G3" s="7" t="s">
         <v>0</v>
       </c>
@@ -30163,25 +30004,25 @@
       </c>
       <c r="J3" s="8"/>
     </row>
-    <row r="4" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="22" t="s">
+    <row r="4" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="23" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="15"/>
-      <c r="C4" s="29" t="s">
-        <v>85</v>
+      <c r="C4" s="19" t="s">
+        <v>39</v>
       </c>
       <c r="D4" s="15"/>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="23" t="s">
         <v>4</v>
       </c>
       <c r="F4" s="15"/>
-      <c r="G4" s="35" t="s">
+      <c r="G4" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="36"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="20"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="30" t="s">
@@ -30197,19 +30038,19 @@
       <c r="I5" s="31"/>
       <c r="J5" s="32"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="30" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="32"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="41"/>
     </row>
     <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
@@ -30218,486 +30059,19 @@
       <c r="B7" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="34" t="s">
+      <c r="C7" s="34"/>
+      <c r="D7" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="20"/>
-      <c r="F7" s="34" t="s">
+      <c r="E7" s="34"/>
+      <c r="F7" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="20"/>
+      <c r="G7" s="34"/>
       <c r="H7" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="20"/>
-      <c r="J7" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="9">
-        <v>1</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="E8" s="15"/>
-      <c r="F8" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="15"/>
-      <c r="H8" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="I8" s="15"/>
-      <c r="J8" s="10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="9">
-        <v>2</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="E9" s="15"/>
-      <c r="F9" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="G9" s="15"/>
-      <c r="H9" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="I9" s="15"/>
-      <c r="J9" s="10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9">
-        <v>3</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="G10" s="15"/>
-      <c r="H10" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="I10" s="15"/>
-      <c r="J10" s="10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9"/>
-      <c r="B11" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="E11" s="37"/>
-      <c r="F11" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="37"/>
-      <c r="H11" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="I11" s="37"/>
-      <c r="J11" s="10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="9">
-        <v>4</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="C12" s="38"/>
-      <c r="D12" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="E12" s="37"/>
-      <c r="F12" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="G12" s="37"/>
-      <c r="H12" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="I12" s="37"/>
-      <c r="J12" s="10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="69" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="9">
-        <v>5</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="C13" s="38"/>
-      <c r="D13" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="E13" s="37"/>
-      <c r="F13" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="G13" s="37"/>
-      <c r="H13" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="I13" s="37"/>
-      <c r="J13" s="10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="9">
-        <v>6</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="C14" s="38"/>
-      <c r="D14" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="E14" s="37"/>
-      <c r="F14" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="G14" s="37"/>
-      <c r="H14" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="I14" s="37"/>
-      <c r="J14" s="10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="9">
-        <v>7</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="E15" s="15"/>
-      <c r="F15" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="G15" s="15"/>
-      <c r="H15" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="I15" s="15"/>
-      <c r="J15" s="10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="9">
-        <v>8</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="15"/>
-      <c r="D16" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="E16" s="15"/>
-      <c r="F16" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="G16" s="15"/>
-      <c r="H16" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="I16" s="15"/>
-      <c r="J16" s="10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="20"/>
-    </row>
-    <row r="18" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="20"/>
-    </row>
-    <row r="19" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="A19" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="21"/>
-      <c r="J19" s="15"/>
-    </row>
-  </sheetData>
-  <mergeCells count="52">
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="B19:J19"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="A17:J17"/>
-    <mergeCell ref="B18:J18"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="A5:J5"/>
-    <mergeCell ref="A6:J6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="A1:J2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:J4"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{D624BFE9-481E-4AEE-8027-953B07977AFD}">
-          <x14:formula1>
-            <xm:f>Parametrización!$B$1:$C$1</xm:f>
-          </x14:formula1>
-          <xm:sqref>H3</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{DA5E4F34-48DC-4E61-A0B0-306225AB73A3}">
-          <x14:formula1>
-            <xm:f>Parametrización!$B$2:$E$2</xm:f>
-          </x14:formula1>
-          <xm:sqref>J8:J16</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4E67FA-54D1-424D-A222-EDE2699A7FA4}">
-  <dimension ref="A1:J16"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="25"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="26"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="28"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="8"/>
-    </row>
-    <row r="4" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="29" t="s">
-        <v>99</v>
-      </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="15"/>
-      <c r="G4" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="36"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="31"/>
-      <c r="J5" s="32"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="32"/>
-    </row>
-    <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="20"/>
-      <c r="F7" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" s="20"/>
-      <c r="H7" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="I7" s="20"/>
+      <c r="I7" s="34"/>
       <c r="J7" s="12" t="s">
         <v>8</v>
       </c>
@@ -30707,28 +30081,28 @@
         <v>1</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
-      <c r="C8" s="15"/>
+      <c r="C8" s="38"/>
       <c r="D8" s="16" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
-      <c r="E8" s="15"/>
-      <c r="F8" s="17" t="s">
-        <v>96</v>
+      <c r="E8" s="21"/>
+      <c r="F8" s="16" t="s">
+        <v>41</v>
       </c>
       <c r="G8" s="15"/>
-      <c r="H8" s="17" t="s">
-        <v>97</v>
+      <c r="H8" s="16" t="s">
+        <v>86</v>
       </c>
-      <c r="I8" s="15"/>
+      <c r="I8" s="21"/>
       <c r="J8" s="10" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="30" t="s">
-        <v>98</v>
+        <v>38</v>
       </c>
       <c r="B9" s="31"/>
       <c r="C9" s="31"/>
@@ -30742,22 +30116,22 @@
     </row>
     <row r="10" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>98</v>
+        <v>38</v>
       </c>
       <c r="C10" s="15"/>
-      <c r="D10" s="16" t="s">
-        <v>100</v>
+      <c r="D10" s="17" t="s">
+        <v>40</v>
       </c>
       <c r="E10" s="15"/>
-      <c r="F10" s="17" t="s">
-        <v>101</v>
+      <c r="F10" s="16" t="s">
+        <v>41</v>
       </c>
       <c r="G10" s="15"/>
-      <c r="H10" s="17" t="s">
-        <v>101</v>
+      <c r="H10" s="16" t="s">
+        <v>41</v>
       </c>
       <c r="I10" s="15"/>
       <c r="J10" s="10" t="s">
@@ -30766,7 +30140,7 @@
     </row>
     <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="39" t="s">
-        <v>103</v>
+        <v>43</v>
       </c>
       <c r="B11" s="31"/>
       <c r="C11" s="31"/>
@@ -30780,22 +30154,22 @@
     </row>
     <row r="12" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>103</v>
+        <v>43</v>
       </c>
       <c r="C12" s="15"/>
-      <c r="D12" s="16" t="s">
-        <v>104</v>
+      <c r="D12" s="17" t="s">
+        <v>44</v>
       </c>
       <c r="E12" s="15"/>
-      <c r="F12" s="17" t="s">
-        <v>101</v>
+      <c r="F12" s="16" t="s">
+        <v>41</v>
       </c>
       <c r="G12" s="15"/>
-      <c r="H12" s="17" t="s">
-        <v>101</v>
+      <c r="H12" s="16" t="s">
+        <v>41</v>
       </c>
       <c r="I12" s="15"/>
       <c r="J12" s="10" t="s">
@@ -30806,66 +30180,98 @@
       <c r="A13" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="20"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="34"/>
     </row>
     <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="20"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="34"/>
     </row>
     <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="9">
         <v>1</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>102</v>
+        <v>42</v>
       </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
       <c r="J15" s="15"/>
     </row>
-    <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="9">
         <v>2</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
       <c r="J16" s="15"/>
     </row>
+    <row r="17" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="A17" s="9">
+        <v>3</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="15"/>
+    </row>
   </sheetData>
-  <mergeCells count="31">
+  <mergeCells count="32">
+    <mergeCell ref="B17:J17"/>
+    <mergeCell ref="B14:J14"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A9:J9"/>
+    <mergeCell ref="A1:J2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="A13:J13"/>
     <mergeCell ref="B16:J16"/>
     <mergeCell ref="A6:J6"/>
     <mergeCell ref="B7:C7"/>
@@ -30882,21 +30288,6 @@
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="H12:I12"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="A13:J13"/>
-    <mergeCell ref="B14:J14"/>
-    <mergeCell ref="A5:J5"/>
-    <mergeCell ref="A9:J9"/>
-    <mergeCell ref="A1:J2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:J4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -30920,7 +30311,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>

</xml_diff>